<commit_message>
use 1011 version 2 cycle benchmark report
</commit_message>
<xml_diff>
--- a/lib/report/benchmark_report/web14/exl/201906/jsliu__bank_test_&_city_(HF)(201906)_Two_Cycles_Comparison.xlsx
+++ b/lib/report/benchmark_report/web14/exl/201906/jsliu__bank_test_&_city_(HF)(201906)_Two_Cycles_Comparison.xlsx
@@ -359,7 +359,7 @@
     <t xml:space="preserve">Bank Name: jsliu  bank test &amp; city (HF)</t>
   </si>
   <si>
-    <t>Printed on: 08/09/19 12:00:48PM</t>
+    <t>Printed on: 10/11/19 7:37:27PM</t>
   </si>
   <si>
     <t xml:space="preserve"> Rate Shock</t>
@@ -754,7 +754,7 @@
     </r>
   </si>
   <si>
-    <t>Printed on: 08/09/19 12:00:42PM</t>
+    <t>Printed on: 10/11/19 7:37:23PM</t>
   </si>
   <si>
     <t xml:space="preserve">Earning/
@@ -3433,7 +3433,7 @@
       <c r="F8" s="124"/>
       <c r="G8" s="124"/>
       <c r="H8" s="124">
-        <v>468.27344305534217</v>
+        <v>486.95327222941927</v>
       </c>
       <c r="I8" s="124"/>
       <c r="J8" s="124"/>
@@ -3445,7 +3445,7 @@
       <c r="N8" s="124"/>
       <c r="O8" s="124"/>
       <c r="P8" s="124">
-        <v>569.43013752531328</v>
+        <v>591.24281219611953</v>
       </c>
       <c r="Q8" s="124"/>
       <c r="R8" s="124"/>
@@ -3481,7 +3481,7 @@
       <c r="AL8" s="124"/>
       <c r="AM8" s="124"/>
       <c r="AN8" s="124">
-        <v>5.874353023896921</v>
+        <v>5.8737311223078494</v>
       </c>
       <c r="AO8" s="124"/>
       <c r="AP8" s="124"/>
@@ -3499,7 +3499,7 @@
       <c r="F9" s="124"/>
       <c r="G9" s="124"/>
       <c r="H9" s="124">
-        <v>351.25927174019915</v>
+        <v>365.04709042354835</v>
       </c>
       <c r="I9" s="124"/>
       <c r="J9" s="124"/>
@@ -3511,7 +3511,7 @@
       <c r="N9" s="124"/>
       <c r="O9" s="124"/>
       <c r="P9" s="124">
-        <v>424.54167130678906</v>
+        <v>440.6853534656172</v>
       </c>
       <c r="Q9" s="124"/>
       <c r="R9" s="124"/>
@@ -3547,7 +3547,7 @@
       <c r="AL9" s="124"/>
       <c r="AM9" s="124"/>
       <c r="AN9" s="124">
-        <v>5.5444482105426527</v>
+        <v>5.5411012728666815</v>
       </c>
       <c r="AO9" s="124"/>
       <c r="AP9" s="124"/>
@@ -3565,7 +3565,7 @@
       <c r="F10" s="124"/>
       <c r="G10" s="124"/>
       <c r="H10" s="124">
-        <v>233.46256126795805</v>
+        <v>242.47366500952805</v>
       </c>
       <c r="I10" s="124"/>
       <c r="J10" s="124"/>
@@ -3577,7 +3577,7 @@
       <c r="N10" s="124"/>
       <c r="O10" s="124"/>
       <c r="P10" s="124">
-        <v>279.122835070389</v>
+        <v>289.65140514706405</v>
       </c>
       <c r="Q10" s="124"/>
       <c r="R10" s="124"/>
@@ -3613,7 +3613,7 @@
       <c r="AL10" s="124"/>
       <c r="AM10" s="124"/>
       <c r="AN10" s="124">
-        <v>5.2123343179186845</v>
+        <v>5.2066479877186485</v>
       </c>
       <c r="AO10" s="124"/>
       <c r="AP10" s="124"/>
@@ -3631,7 +3631,7 @@
       <c r="F11" s="124"/>
       <c r="G11" s="124"/>
       <c r="H11" s="124">
-        <v>114.78847494649239</v>
+        <v>119.1462972003761</v>
       </c>
       <c r="I11" s="124"/>
       <c r="J11" s="124"/>
@@ -3643,7 +3643,7 @@
       <c r="N11" s="124"/>
       <c r="O11" s="124"/>
       <c r="P11" s="124">
-        <v>133.10567519986506</v>
+        <v>138.09140740176957</v>
       </c>
       <c r="Q11" s="124"/>
       <c r="R11" s="124"/>
@@ -3679,7 +3679,7 @@
       <c r="AL11" s="124"/>
       <c r="AM11" s="124"/>
       <c r="AN11" s="124">
-        <v>4.8777489507845013</v>
+        <v>4.8701396869399325</v>
       </c>
       <c r="AO11" s="124"/>
       <c r="AP11" s="124"/>
@@ -3745,7 +3745,7 @@
       <c r="AL12" s="124"/>
       <c r="AM12" s="124"/>
       <c r="AN12" s="124">
-        <v>4.5541238999171449</v>
+        <v>4.5450451352843553</v>
       </c>
       <c r="AO12" s="124"/>
       <c r="AP12" s="124"/>
@@ -3763,7 +3763,7 @@
       <c r="F13" s="124"/>
       <c r="G13" s="124"/>
       <c r="H13" s="124">
-        <v>-71.243966332150364</v>
+        <v>-73.948966369147072</v>
       </c>
       <c r="I13" s="124"/>
       <c r="J13" s="124"/>
@@ -3775,7 +3775,7 @@
       <c r="N13" s="124"/>
       <c r="O13" s="124"/>
       <c r="P13" s="124">
-        <v>-80.574059823532664</v>
+        <v>-83.596663990059255</v>
       </c>
       <c r="Q13" s="124"/>
       <c r="R13" s="124"/>
@@ -3811,7 +3811,7 @@
       <c r="AL13" s="124"/>
       <c r="AM13" s="124"/>
       <c r="AN13" s="124">
-        <v>4.3532783683369329</v>
+        <v>4.3432867366126464</v>
       </c>
       <c r="AO13" s="124"/>
       <c r="AP13" s="124"/>
@@ -3829,7 +3829,7 @@
       <c r="F14" s="124"/>
       <c r="G14" s="124"/>
       <c r="H14" s="124">
-        <v>-82.726987115066621</v>
+        <v>-86.712084986110725</v>
       </c>
       <c r="I14" s="124"/>
       <c r="J14" s="124"/>
@@ -3841,7 +3841,7 @@
       <c r="N14" s="124"/>
       <c r="O14" s="124"/>
       <c r="P14" s="124">
-        <v>-89.345284951847631</v>
+        <v>-93.213890326165853</v>
       </c>
       <c r="Q14" s="124"/>
       <c r="R14" s="124"/>
@@ -3877,7 +3877,7 @@
       <c r="AL14" s="124"/>
       <c r="AM14" s="124"/>
       <c r="AN14" s="124">
-        <v>4.3209265525276166</v>
+        <v>4.3084845263129665</v>
       </c>
       <c r="AO14" s="124"/>
       <c r="AP14" s="124"/>
@@ -3941,7 +3941,7 @@
       <c r="F16" s="124"/>
       <c r="G16" s="124"/>
       <c r="H16" s="124">
-        <v>-76.470925606337261</v>
+        <v>-79.043577675263066</v>
       </c>
       <c r="I16" s="124"/>
       <c r="J16" s="124"/>
@@ -3953,7 +3953,7 @@
       <c r="N16" s="124"/>
       <c r="O16" s="124"/>
       <c r="P16" s="124">
-        <v>-99.374001099234476</v>
+        <v>-102.63073764166167</v>
       </c>
       <c r="Q16" s="124"/>
       <c r="R16" s="124"/>
@@ -3989,7 +3989,7 @@
       <c r="AL16" s="124"/>
       <c r="AM16" s="124"/>
       <c r="AN16" s="124">
-        <v>4.3385650496449371</v>
+        <v>4.3294090896351873</v>
       </c>
       <c r="AO16" s="124"/>
       <c r="AP16" s="124"/>
@@ -4007,7 +4007,7 @@
       <c r="F17" s="124"/>
       <c r="G17" s="124"/>
       <c r="H17" s="124">
-        <v>347.7293174430713</v>
+        <v>361.6225358433415</v>
       </c>
       <c r="I17" s="124"/>
       <c r="J17" s="124"/>
@@ -4019,7 +4019,7 @@
       <c r="N17" s="124"/>
       <c r="O17" s="124"/>
       <c r="P17" s="124">
-        <v>386.63006451086051</v>
+        <v>401.57626450132381</v>
       </c>
       <c r="Q17" s="124"/>
       <c r="R17" s="124"/>
@@ -4055,7 +4055,7 @@
       <c r="AL17" s="124"/>
       <c r="AM17" s="124"/>
       <c r="AN17" s="124">
-        <v>5.5344977076652038</v>
+        <v>5.5317588428607785</v>
       </c>
       <c r="AO17" s="124"/>
       <c r="AP17" s="124"/>
@@ -4271,13 +4271,13 @@
       <c r="F23" s="106"/>
       <c r="G23" s="106"/>
       <c r="H23" s="106">
-        <v>-231.245579442238</v>
+        <v>-223.79927007370162</v>
       </c>
       <c r="I23" s="106"/>
       <c r="J23" s="106"/>
       <c r="K23" s="106"/>
       <c r="L23" s="106">
-        <v>-4638.9363147489294</v>
+        <v>-4631.4900053803931</v>
       </c>
       <c r="M23" s="106"/>
       <c r="N23" s="106"/>
@@ -4311,7 +4311,7 @@
       <c r="AL23" s="106"/>
       <c r="AM23" s="106"/>
       <c r="AN23" s="106">
-        <v>-2517.4556290896021</v>
+        <v>-2510.0093197210658</v>
       </c>
       <c r="AO23" s="106"/>
       <c r="AP23" s="106"/>
@@ -4329,13 +4329,13 @@
       <c r="F24" s="106"/>
       <c r="G24" s="106"/>
       <c r="H24" s="106">
-        <v>-454.48319091922912</v>
+        <v>-439.79001070509332</v>
       </c>
       <c r="I24" s="106"/>
       <c r="J24" s="106"/>
       <c r="K24" s="106"/>
       <c r="L24" s="106">
-        <v>-8780.5104830143264</v>
+        <v>-8765.8173028001911</v>
       </c>
       <c r="M24" s="106"/>
       <c r="N24" s="106"/>
@@ -4369,7 +4369,7 @@
       <c r="AL24" s="106"/>
       <c r="AM24" s="106"/>
       <c r="AN24" s="106">
-        <v>-4537.5491116956719</v>
+        <v>-4522.8559314815366</v>
       </c>
       <c r="AO24" s="106"/>
       <c r="AP24" s="106"/>
@@ -4387,13 +4387,13 @@
       <c r="F25" s="106"/>
       <c r="G25" s="106"/>
       <c r="H25" s="106">
-        <v>-3001.6568079842145</v>
+        <v>-2995.6729269421121</v>
       </c>
       <c r="I25" s="106"/>
       <c r="J25" s="106"/>
       <c r="K25" s="106"/>
       <c r="L25" s="106">
-        <v>-3673.4235913653642</v>
+        <v>-3667.4397103232614</v>
       </c>
       <c r="M25" s="106"/>
       <c r="N25" s="106"/>
@@ -4427,13 +4427,13 @@
       <c r="AH25" s="106"/>
       <c r="AI25" s="106"/>
       <c r="AJ25" s="106">
-        <v>897.51272338356739</v>
+        <v>896.05029505713367</v>
       </c>
       <c r="AK25" s="106"/>
       <c r="AL25" s="106"/>
       <c r="AM25" s="106"/>
       <c r="AN25" s="106">
-        <v>-2517.4556290896044</v>
+        <v>-2510.0093197210681</v>
       </c>
       <c r="AO25" s="106"/>
       <c r="AP25" s="106"/>
@@ -4451,13 +4451,13 @@
       <c r="F26" s="106"/>
       <c r="G26" s="106"/>
       <c r="H26" s="106">
-        <v>-5996.8783840540136</v>
+        <v>-5985.0708914855395</v>
       </c>
       <c r="I26" s="106"/>
       <c r="J26" s="106"/>
       <c r="K26" s="106"/>
       <c r="L26" s="106">
-        <v>-6947.0464765458428</v>
+        <v>-6935.2389839773678</v>
       </c>
       <c r="M26" s="106"/>
       <c r="N26" s="106"/>
@@ -4491,13 +4491,13 @@
       <c r="AH26" s="106"/>
       <c r="AI26" s="106"/>
       <c r="AJ26" s="106">
-        <v>1697.4640064684841</v>
+        <v>1694.5783188228249</v>
       </c>
       <c r="AK26" s="106"/>
       <c r="AL26" s="106"/>
       <c r="AM26" s="106"/>
       <c r="AN26" s="106">
-        <v>-4537.5491116956719</v>
+        <v>-4522.8559314815384</v>
       </c>
       <c r="AO26" s="106"/>
       <c r="AP26" s="106"/>
@@ -6827,7 +6827,7 @@
       </c>
       <c r="Y56" s="140"/>
       <c r="Z56" s="141">
-        <v>38.1036509417304</v>
+        <v>38.1036509417303</v>
       </c>
       <c r="AA56" s="141"/>
       <c r="AB56" s="141"/>
@@ -6837,15 +6837,15 @@
       <c r="AD56" s="141"/>
       <c r="AE56" s="141"/>
       <c r="AF56" s="140">
-        <v>118.8026628039172</v>
+        <v>118.80266280391689</v>
       </c>
       <c r="AG56" s="140"/>
       <c r="AH56" s="140">
-        <v>-10.533788030045466</v>
+        <v>-10.533788030045232</v>
       </c>
       <c r="AI56" s="140"/>
       <c r="AJ56" s="140">
-        <v>1.74712941973342</v>
+        <v>1.74712941973343</v>
       </c>
       <c r="AK56" s="140"/>
       <c r="AL56" s="140">
@@ -6853,7 +6853,7 @@
       </c>
       <c r="AM56" s="140"/>
       <c r="AN56" s="140">
-        <v>-0.8287669139606002</v>
+        <v>-0.82876691396059021</v>
       </c>
       <c r="AO56" s="140"/>
       <c r="AP56" s="141">
@@ -6861,7 +6861,7 @@
       </c>
       <c r="AQ56" s="141"/>
       <c r="AR56" s="141">
-        <v>1.822738998292005</v>
+        <v>1.8227389982919047</v>
       </c>
       <c r="AS56" s="141"/>
       <c r="AT56" s="141">
@@ -6875,7 +6875,7 @@
         <v>-0.19180153977603759</v>
       </c>
       <c r="AX56" s="142">
-        <v>0.047836334661983157</v>
+        <v>0.047836334661980652</v>
       </c>
       <c r="AY56" s="142">
         <v>0</v>
@@ -6884,7 +6884,7 @@
         <v>0.7136137967076055</v>
       </c>
       <c r="BA56" s="142">
-        <v>-0.47435920006833548</v>
+        <v>-0.47435920006832705</v>
       </c>
     </row>
     <row r="57">
@@ -6953,7 +6953,7 @@
       </c>
       <c r="AI57" s="140"/>
       <c r="AJ57" s="140">
-        <v>4.45578905757086</v>
+        <v>4.45578905757172</v>
       </c>
       <c r="AK57" s="140"/>
       <c r="AL57" s="140">
@@ -6961,7 +6961,7 @@
       </c>
       <c r="AM57" s="140"/>
       <c r="AN57" s="140">
-        <v>1.8798927238776004</v>
+        <v>1.8798927238784602</v>
       </c>
       <c r="AO57" s="140"/>
       <c r="AP57" s="141">
@@ -6992,7 +6992,7 @@
         <v>0.46300832925036811</v>
       </c>
       <c r="BA57" s="142">
-        <v>0.42189894979060161</v>
+        <v>0.42189894979071313</v>
       </c>
     </row>
     <row r="58">
@@ -7043,7 +7043,7 @@
       </c>
       <c r="Y58" s="148"/>
       <c r="Z58" s="149">
-        <v>91.766658768599</v>
+        <v>91.7666587685989</v>
       </c>
       <c r="AA58" s="149"/>
       <c r="AB58" s="149"/>
@@ -7053,15 +7053,15 @@
       <c r="AD58" s="149"/>
       <c r="AE58" s="149"/>
       <c r="AF58" s="148">
-        <v>111.31154981051935</v>
+        <v>111.31154981051922</v>
       </c>
       <c r="AG58" s="148"/>
       <c r="AH58" s="148">
-        <v>-13.861496054060705</v>
+        <v>-13.861496054060611</v>
       </c>
       <c r="AI58" s="148"/>
       <c r="AJ58" s="148">
-        <v>3.33109058053062</v>
+        <v>3.33109058053116</v>
       </c>
       <c r="AK58" s="148"/>
       <c r="AL58" s="148">
@@ -7069,7 +7069,7 @@
       </c>
       <c r="AM58" s="148"/>
       <c r="AN58" s="148">
-        <v>0.75519424683709024</v>
+        <v>0.75519424683763026</v>
       </c>
       <c r="AO58" s="148"/>
       <c r="AP58" s="149">
@@ -7077,7 +7077,7 @@
       </c>
       <c r="AQ58" s="149"/>
       <c r="AR58" s="149">
-        <v>-1.4905621723822031</v>
+        <v>-1.4905621723823086</v>
       </c>
       <c r="AS58" s="149"/>
       <c r="AT58" s="149">
@@ -7091,7 +7091,7 @@
         <v>-0.50471144426373316</v>
       </c>
       <c r="AX58" s="150">
-        <v>-0.016242960050892125</v>
+        <v>-0.016242960050893294</v>
       </c>
       <c r="AY58" s="150">
         <v>0</v>
@@ -7100,7 +7100,7 @@
         <v>0.60589715929521781</v>
       </c>
       <c r="BA58" s="150">
-        <v>0.22671081094312148</v>
+        <v>0.22671081094324685</v>
       </c>
     </row>
     <row r="59">
@@ -8881,7 +8881,7 @@
       </c>
       <c r="AI75" s="148"/>
       <c r="AJ75" s="148">
-        <v>2.1133528313297</v>
+        <v>2.11335283132976</v>
       </c>
       <c r="AK75" s="148"/>
       <c r="AL75" s="148">
@@ -8889,7 +8889,7 @@
       </c>
       <c r="AM75" s="148"/>
       <c r="AN75" s="148">
-        <v>0.6000775676855401</v>
+        <v>0.6000775676856</v>
       </c>
       <c r="AO75" s="148"/>
       <c r="AP75" s="149">
@@ -8920,7 +8920,7 @@
         <v>-0.45130142737196377</v>
       </c>
       <c r="BA75" s="150">
-        <v>0.28394575614142831</v>
+        <v>0.28394575614144862</v>
       </c>
     </row>
     <row r="76">
@@ -11279,55 +11279,55 @@
       </c>
       <c r="C111" s="4"/>
       <c r="D111" s="106">
-        <v>-39.943078732896623</v>
+        <v>-29.738256809098015</v>
       </c>
       <c r="E111" s="106"/>
       <c r="F111" s="106"/>
       <c r="G111" s="106"/>
       <c r="H111" s="106">
-        <v>-66.497056679823928</v>
+        <v>-58.302023112503385</v>
       </c>
       <c r="I111" s="106"/>
       <c r="J111" s="106"/>
       <c r="K111" s="106"/>
       <c r="L111" s="106">
-        <v>-231.245579442238</v>
+        <v>-223.79927007370162</v>
       </c>
       <c r="M111" s="106"/>
       <c r="N111" s="106"/>
       <c r="O111" s="106"/>
       <c r="P111" s="106">
-        <v>-496.68885346516248</v>
+        <v>-490.44781352798651</v>
       </c>
       <c r="Q111" s="106"/>
       <c r="R111" s="106"/>
       <c r="S111" s="106"/>
       <c r="T111" s="106">
-        <v>-771.11743202701746</v>
+        <v>-766.45356248597784</v>
       </c>
       <c r="U111" s="106"/>
       <c r="V111" s="106"/>
       <c r="W111" s="106"/>
       <c r="X111" s="106">
-        <v>-1043.517117722447</v>
+        <v>-1040.7719938668884</v>
       </c>
       <c r="Y111" s="106"/>
       <c r="Z111" s="106"/>
       <c r="AA111" s="106"/>
       <c r="AB111" s="106">
-        <v>-1314.1072162096823</v>
+        <v>-1313.5971389231472</v>
       </c>
       <c r="AC111" s="106"/>
       <c r="AD111" s="106"/>
       <c r="AE111" s="106"/>
       <c r="AF111" s="106">
-        <v>-1035.3542544540073</v>
+        <v>-1033.10786571311</v>
       </c>
       <c r="AG111" s="106"/>
       <c r="AH111" s="106"/>
       <c r="AI111" s="106"/>
       <c r="AJ111" s="105">
-        <v>114.78847494649239</v>
+        <v>119.1462972003761</v>
       </c>
       <c r="AK111" s="105"/>
       <c r="AL111" s="105"/>
@@ -12239,42 +12239,42 @@
       <c r="Q127" s="102"/>
       <c r="R127" s="102"/>
       <c r="S127" s="102">
-        <v>23.9501805327689</v>
+        <v>23.7334629925411</v>
       </c>
       <c r="T127" s="102"/>
       <c r="U127" s="102"/>
       <c r="V127" s="102">
-        <v>23.468577069242603</v>
+        <v>23.5066908303199</v>
       </c>
       <c r="W127" s="102"/>
       <c r="X127" s="102"/>
       <c r="Y127" s="102">
-        <v>23.0259294553914</v>
+        <v>23.266306149136998</v>
       </c>
       <c r="Z127" s="102"/>
       <c r="AA127" s="102"/>
       <c r="AB127" s="102">
-        <v>22.5843635821507</v>
+        <v>23.0199105548528</v>
       </c>
       <c r="AC127" s="102"/>
       <c r="AD127" s="102"/>
       <c r="AE127" s="102">
-        <v>22.1802641755488</v>
+        <v>22.811299056808398</v>
       </c>
       <c r="AF127" s="102"/>
       <c r="AG127" s="102"/>
       <c r="AH127" s="102">
-        <v>21.8245350392199</v>
+        <v>22.5711842379646</v>
       </c>
       <c r="AI127" s="102"/>
       <c r="AJ127" s="102"/>
       <c r="AK127" s="102">
-        <v>21.7928975726436</v>
+        <v>22.7346591537199</v>
       </c>
       <c r="AL127" s="102"/>
       <c r="AM127" s="102"/>
       <c r="AN127" s="102">
-        <v>20.6425524922044</v>
+        <v>21.6120939713776</v>
       </c>
       <c r="AO127" s="102"/>
       <c r="AP127" s="102"/>
@@ -12365,42 +12365,42 @@
       <c r="Q129" s="100"/>
       <c r="R129" s="100"/>
       <c r="S129" s="100">
-        <v>-21.8956281267881</v>
+        <v>-22.112345667015802</v>
       </c>
       <c r="T129" s="100"/>
       <c r="U129" s="100"/>
       <c r="V129" s="100">
-        <v>-20.0411958913794</v>
+        <v>-20.0030821303021</v>
       </c>
       <c r="W129" s="100"/>
       <c r="X129" s="100"/>
       <c r="Y129" s="100">
-        <v>-18.4775837252878</v>
+        <v>-18.237207031542198</v>
       </c>
       <c r="Z129" s="100"/>
       <c r="AA129" s="100"/>
       <c r="AB129" s="100">
-        <v>-18.5628732390847</v>
+        <v>-18.127326266382703</v>
       </c>
       <c r="AC129" s="100"/>
       <c r="AD129" s="100"/>
       <c r="AE129" s="100">
-        <v>-18.859902342534998</v>
+        <v>-18.2288674612754</v>
       </c>
       <c r="AF129" s="100"/>
       <c r="AG129" s="100"/>
       <c r="AH129" s="100">
-        <v>-18.726914150082298</v>
+        <v>-17.980264951337602</v>
       </c>
       <c r="AI129" s="100"/>
       <c r="AJ129" s="100"/>
       <c r="AK129" s="100">
-        <v>-17.9688835210771</v>
+        <v>-17.0271219400008</v>
       </c>
       <c r="AL129" s="100"/>
       <c r="AM129" s="100"/>
       <c r="AN129" s="100">
-        <v>-18.4171390023042</v>
+        <v>-17.4475975231309</v>
       </c>
       <c r="AO129" s="100"/>
       <c r="AP129" s="100"/>
@@ -12554,42 +12554,42 @@
       <c r="Q132" s="100"/>
       <c r="R132" s="100"/>
       <c r="S132" s="100">
-        <v>-313.895628126788</v>
+        <v>-314.112345667016</v>
       </c>
       <c r="T132" s="100"/>
       <c r="U132" s="100"/>
       <c r="V132" s="100">
-        <v>-312.04119589137895</v>
+        <v>-312.003082130302</v>
       </c>
       <c r="W132" s="100"/>
       <c r="X132" s="100"/>
       <c r="Y132" s="100">
-        <v>-310.477583725288</v>
+        <v>-310.237207031542</v>
       </c>
       <c r="Z132" s="100"/>
       <c r="AA132" s="100"/>
       <c r="AB132" s="100">
-        <v>-310.56287323908504</v>
+        <v>-310.127326266383</v>
       </c>
       <c r="AC132" s="100"/>
       <c r="AD132" s="100"/>
       <c r="AE132" s="100">
-        <v>-310.85990234253495</v>
+        <v>-310.228867461275</v>
       </c>
       <c r="AF132" s="100"/>
       <c r="AG132" s="100"/>
       <c r="AH132" s="100">
-        <v>-310.726914150082</v>
+        <v>-309.98026495133803</v>
       </c>
       <c r="AI132" s="100"/>
       <c r="AJ132" s="100"/>
       <c r="AK132" s="100">
-        <v>-309.968883521077</v>
+        <v>-309.027121940001</v>
       </c>
       <c r="AL132" s="100"/>
       <c r="AM132" s="100"/>
       <c r="AN132" s="100">
-        <v>-310.417139002304</v>
+        <v>-309.447597523131</v>
       </c>
       <c r="AO132" s="100"/>
       <c r="AP132" s="100"/>
@@ -12617,42 +12617,42 @@
       <c r="Q133" s="100"/>
       <c r="R133" s="100"/>
       <c r="S133" s="100">
-        <v>-61.6479702086844</v>
+        <v>-61.690532752621</v>
       </c>
       <c r="T133" s="100"/>
       <c r="U133" s="100"/>
       <c r="V133" s="100">
-        <v>-61.2837664002888</v>
+        <v>-61.276280994960096</v>
       </c>
       <c r="W133" s="100"/>
       <c r="X133" s="100"/>
       <c r="Y133" s="100">
-        <v>-60.976678605506905</v>
+        <v>-60.9294694890775</v>
       </c>
       <c r="Z133" s="100"/>
       <c r="AA133" s="100"/>
       <c r="AB133" s="100">
-        <v>-60.993429158667</v>
+        <v>-60.9078893027669</v>
       </c>
       <c r="AC133" s="100"/>
       <c r="AD133" s="100"/>
       <c r="AE133" s="100">
-        <v>-61.0517646042095</v>
+        <v>-60.9278316275296</v>
       </c>
       <c r="AF133" s="100"/>
       <c r="AG133" s="100"/>
       <c r="AH133" s="100">
-        <v>-61.0256462024485</v>
+        <v>-60.879006990442804</v>
       </c>
       <c r="AI133" s="100"/>
       <c r="AJ133" s="100"/>
       <c r="AK133" s="100">
-        <v>-60.8767717185538</v>
+        <v>-60.6918131377658</v>
       </c>
       <c r="AL133" s="100"/>
       <c r="AM133" s="100"/>
       <c r="AN133" s="100">
-        <v>-60.964807479731704</v>
+        <v>-60.7743930270652</v>
       </c>
       <c r="AO133" s="100"/>
       <c r="AP133" s="100"/>
@@ -12680,42 +12680,42 @@
       <c r="Q134" s="100"/>
       <c r="R134" s="100"/>
       <c r="S134" s="100">
-        <v>-252.247657918104</v>
+        <v>-252.42181291439502</v>
       </c>
       <c r="T134" s="100"/>
       <c r="U134" s="100"/>
       <c r="V134" s="100">
-        <v>-250.757429491091</v>
+        <v>-250.726801135342</v>
       </c>
       <c r="W134" s="100"/>
       <c r="X134" s="100"/>
       <c r="Y134" s="100">
-        <v>-249.500905119781</v>
+        <v>-249.30773754246502</v>
       </c>
       <c r="Z134" s="100"/>
       <c r="AA134" s="100"/>
       <c r="AB134" s="100">
-        <v>-249.569444080418</v>
+        <v>-249.219436963616</v>
       </c>
       <c r="AC134" s="100"/>
       <c r="AD134" s="100"/>
       <c r="AE134" s="100">
-        <v>-249.80813773832603</v>
+        <v>-249.301035833746</v>
       </c>
       <c r="AF134" s="100"/>
       <c r="AG134" s="100"/>
       <c r="AH134" s="100">
-        <v>-249.70126794763402</v>
+        <v>-249.101257960895</v>
       </c>
       <c r="AI134" s="100"/>
       <c r="AJ134" s="100"/>
       <c r="AK134" s="100">
-        <v>-249.092111802523</v>
+        <v>-248.335308802235</v>
       </c>
       <c r="AL134" s="100"/>
       <c r="AM134" s="100"/>
       <c r="AN134" s="100">
-        <v>-249.452331522572</v>
+        <v>-248.673204496066</v>
       </c>
       <c r="AO134" s="100"/>
       <c r="AP134" s="100"/>
@@ -12745,42 +12745,42 @@
       <c r="Q135" s="100"/>
       <c r="R135" s="100"/>
       <c r="S135" s="100">
-        <v>-69132.563344437411</v>
+        <v>-69132.737499433613</v>
       </c>
       <c r="T135" s="100"/>
       <c r="U135" s="100"/>
       <c r="V135" s="100">
-        <v>-69383.320773927</v>
+        <v>-69383.4643005676</v>
       </c>
       <c r="W135" s="100"/>
       <c r="X135" s="100"/>
       <c r="Y135" s="100">
-        <v>-69632.8216790482</v>
+        <v>-69632.772038111492</v>
       </c>
       <c r="Z135" s="100"/>
       <c r="AA135" s="100"/>
       <c r="AB135" s="100">
-        <v>-69882.391123128691</v>
+        <v>-69881.99147507509</v>
       </c>
       <c r="AC135" s="100"/>
       <c r="AD135" s="100"/>
       <c r="AE135" s="100">
-        <v>-70132.19926086851</v>
+        <v>-70131.292510910309</v>
       </c>
       <c r="AF135" s="100"/>
       <c r="AG135" s="100"/>
       <c r="AH135" s="100">
-        <v>-70381.9005288147</v>
+        <v>-70380.3937688698</v>
       </c>
       <c r="AI135" s="100"/>
       <c r="AJ135" s="100"/>
       <c r="AK135" s="100">
-        <v>-70630.992640618613</v>
+        <v>-70628.729077673488</v>
       </c>
       <c r="AL135" s="100"/>
       <c r="AM135" s="100"/>
       <c r="AN135" s="100">
-        <v>-70880.4449721426</v>
+        <v>-70877.402282170908</v>
       </c>
       <c r="AO135" s="100"/>
       <c r="AP135" s="100"/>
@@ -12901,13 +12901,13 @@
       <c r="F141" s="158"/>
       <c r="G141" s="158"/>
       <c r="H141" s="158">
-        <v>3074.39877694932</v>
+        <v>3077.63347475744</v>
       </c>
       <c r="I141" s="158"/>
       <c r="J141" s="158"/>
       <c r="K141" s="158"/>
       <c r="L141" s="158">
-        <v>-5945.65756869006</v>
+        <v>-5942.42287088194</v>
       </c>
       <c r="M141" s="158"/>
       <c r="N141" s="158"/>
@@ -12919,13 +12919,13 @@
       <c r="R141" s="158"/>
       <c r="S141" s="158"/>
       <c r="T141" s="158">
-        <v>1455.27623778888</v>
+        <v>1461.6589967478099</v>
       </c>
       <c r="U141" s="158"/>
       <c r="V141" s="158"/>
       <c r="W141" s="158"/>
       <c r="X141" s="158">
-        <v>-7769.9470505653189</v>
+        <v>-7763.56429160639</v>
       </c>
       <c r="Y141" s="158"/>
       <c r="Z141" s="158"/>
@@ -12943,13 +12943,13 @@
       <c r="F142" s="158"/>
       <c r="G142" s="158"/>
       <c r="H142" s="158">
-        <v>2612.94441506955</v>
+        <v>2615.69359830353</v>
       </c>
       <c r="I142" s="158"/>
       <c r="J142" s="158"/>
       <c r="K142" s="158"/>
       <c r="L142" s="158">
-        <v>-606.76602009533019</v>
+        <v>-604.01683686135016</v>
       </c>
       <c r="M142" s="158"/>
       <c r="N142" s="158"/>
@@ -12961,13 +12961,13 @@
       <c r="R142" s="158"/>
       <c r="S142" s="158"/>
       <c r="T142" s="158">
-        <v>1236.8453781675999</v>
+        <v>1242.27011177715</v>
       </c>
       <c r="U142" s="158"/>
       <c r="V142" s="158"/>
       <c r="W142" s="158"/>
       <c r="X142" s="158">
-        <v>-2056.09942728247</v>
+        <v>-2050.67469367292</v>
       </c>
       <c r="Y142" s="158"/>
       <c r="Z142" s="158"/>
@@ -12985,13 +12985,13 @@
       <c r="F143" s="160"/>
       <c r="G143" s="160"/>
       <c r="H143" s="160">
-        <v>5687.3431920188705</v>
+        <v>5693.32707306097</v>
       </c>
       <c r="I143" s="160"/>
       <c r="J143" s="160"/>
       <c r="K143" s="160"/>
       <c r="L143" s="160">
-        <v>-6552.42358878543</v>
+        <v>-6546.4397077433305</v>
       </c>
       <c r="M143" s="160"/>
       <c r="N143" s="160"/>
@@ -13003,13 +13003,13 @@
       <c r="R143" s="160"/>
       <c r="S143" s="160"/>
       <c r="T143" s="160">
-        <v>2692.12161595648</v>
+        <v>2703.92910852496</v>
       </c>
       <c r="U143" s="160"/>
       <c r="V143" s="160"/>
       <c r="W143" s="160"/>
       <c r="X143" s="160">
-        <v>-9826.04647784782</v>
+        <v>-9814.23898527934</v>
       </c>
       <c r="Y143" s="160"/>
       <c r="Z143" s="160"/>
@@ -14451,13 +14451,13 @@
       <c r="F178" s="160"/>
       <c r="G178" s="160"/>
       <c r="H178" s="160">
-        <v>12588.4068950503</v>
+        <v>12594.390776092401</v>
       </c>
       <c r="I178" s="160"/>
       <c r="J178" s="160"/>
       <c r="K178" s="160"/>
       <c r="L178" s="160">
-        <v>-91313.3598857537</v>
+        <v>-91307.3760047116</v>
       </c>
       <c r="M178" s="160"/>
       <c r="N178" s="160"/>
@@ -14469,13 +14469,13 @@
       <c r="R178" s="160"/>
       <c r="S178" s="160"/>
       <c r="T178" s="160">
-        <v>9593.1853189879512</v>
+        <v>9604.99281155642</v>
       </c>
       <c r="U178" s="160"/>
       <c r="V178" s="160"/>
       <c r="W178" s="160"/>
       <c r="X178" s="160">
-        <v>-94586.982774816046</v>
+        <v>-94575.175282247583</v>
       </c>
       <c r="Y178" s="160"/>
       <c r="Z178" s="160"/>
@@ -14867,13 +14867,13 @@
       <c r="F190" s="160"/>
       <c r="G190" s="160"/>
       <c r="H190" s="160">
-        <v>-71628.551438283</v>
+        <v>-71622.567557240909</v>
       </c>
       <c r="I190" s="160"/>
       <c r="J190" s="160"/>
       <c r="K190" s="160"/>
       <c r="L190" s="160">
-        <v>-83864.3182190872</v>
+        <v>-83858.3343380451</v>
       </c>
       <c r="M190" s="160"/>
       <c r="N190" s="160"/>
@@ -14885,13 +14885,13 @@
       <c r="R190" s="160"/>
       <c r="S190" s="160"/>
       <c r="T190" s="160">
-        <v>-74623.7730143454</v>
+        <v>-74611.9655217769</v>
       </c>
       <c r="U190" s="160"/>
       <c r="V190" s="160"/>
       <c r="W190" s="160"/>
       <c r="X190" s="160">
-        <v>-87137.9411081497</v>
+        <v>-87126.1336155812</v>
       </c>
       <c r="Y190" s="160"/>
       <c r="Z190" s="160"/>
@@ -15111,13 +15111,13 @@
       <c r="F197" s="158"/>
       <c r="G197" s="158"/>
       <c r="H197" s="158">
-        <v>70382.396229797669</v>
+        <v>77828.705598333865</v>
       </c>
       <c r="I197" s="158"/>
       <c r="J197" s="158"/>
       <c r="K197" s="158"/>
       <c r="L197" s="158">
-        <v>-7725.269006703762</v>
+        <v>-278.95963816756557</v>
       </c>
       <c r="M197" s="158"/>
       <c r="N197" s="158"/>
@@ -15129,13 +15129,13 @@
       <c r="R197" s="158"/>
       <c r="S197" s="158"/>
       <c r="T197" s="158">
-        <v>33396.8854813406</v>
+        <v>40643.756326939627</v>
       </c>
       <c r="U197" s="158"/>
       <c r="V197" s="158"/>
       <c r="W197" s="158"/>
       <c r="X197" s="158">
-        <v>-37553.071179365761</v>
+        <v>-30306.200333766734</v>
       </c>
       <c r="Y197" s="158"/>
       <c r="Z197" s="158"/>
@@ -15153,13 +15153,13 @@
       <c r="F198" s="160"/>
       <c r="G198" s="160"/>
       <c r="H198" s="160">
-        <v>70382.396229797669</v>
+        <v>77828.705598333865</v>
       </c>
       <c r="I198" s="160"/>
       <c r="J198" s="160"/>
       <c r="K198" s="160"/>
       <c r="L198" s="160">
-        <v>-7725.269006703762</v>
+        <v>-278.95963816756557</v>
       </c>
       <c r="M198" s="160"/>
       <c r="N198" s="160"/>
@@ -15171,13 +15171,13 @@
       <c r="R198" s="160"/>
       <c r="S198" s="160"/>
       <c r="T198" s="160">
-        <v>33396.8854813406</v>
+        <v>40643.756326939627</v>
       </c>
       <c r="U198" s="160"/>
       <c r="V198" s="160"/>
       <c r="W198" s="160"/>
       <c r="X198" s="160">
-        <v>-37553.071179365761</v>
+        <v>-30306.200333766734</v>
       </c>
       <c r="Y198" s="160"/>
       <c r="Z198" s="160"/>
@@ -16619,13 +16619,13 @@
       <c r="F233" s="160"/>
       <c r="G233" s="160"/>
       <c r="H233" s="160">
-        <v>265619.27085571259</v>
+        <v>273065.58022424887</v>
       </c>
       <c r="I233" s="160"/>
       <c r="J233" s="160"/>
       <c r="K233" s="160"/>
       <c r="L233" s="160">
-        <v>-4890347.805869625</v>
+        <v>-4882901.4965010891</v>
       </c>
       <c r="M233" s="160"/>
       <c r="N233" s="160"/>
@@ -16637,13 +16637,13 @@
       <c r="R233" s="160"/>
       <c r="S233" s="160"/>
       <c r="T233" s="160">
-        <v>210370.08954861396</v>
+        <v>217616.96039421292</v>
       </c>
       <c r="U233" s="160"/>
       <c r="V233" s="160"/>
       <c r="W233" s="160"/>
       <c r="X233" s="160">
-        <v>-4597529.130870292</v>
+        <v>-4590282.2600246929</v>
       </c>
       <c r="Y233" s="160"/>
       <c r="Z233" s="160"/>
@@ -17035,13 +17035,13 @@
       <c r="F245" s="160"/>
       <c r="G245" s="160"/>
       <c r="H245" s="160">
-        <v>-231245.579442238</v>
+        <v>-223799.27007370163</v>
       </c>
       <c r="I245" s="160"/>
       <c r="J245" s="160"/>
       <c r="K245" s="160"/>
       <c r="L245" s="160">
-        <v>-4638936.31474893</v>
+        <v>-4631490.005380393</v>
       </c>
       <c r="M245" s="160"/>
       <c r="N245" s="160"/>
@@ -17053,13 +17053,13 @@
       <c r="R245" s="160"/>
       <c r="S245" s="160"/>
       <c r="T245" s="160">
-        <v>-223237.61147699109</v>
+        <v>-215990.7406313917</v>
       </c>
       <c r="U245" s="160"/>
       <c r="V245" s="160"/>
       <c r="W245" s="160"/>
       <c r="X245" s="160">
-        <v>-4141574.1682653958</v>
+        <v>-4134327.2974197967</v>
       </c>
       <c r="Y245" s="160"/>
       <c r="Z245" s="160"/>
@@ -17283,13 +17283,13 @@
       <c r="F252" s="153"/>
       <c r="G252" s="153"/>
       <c r="H252" s="153">
-        <v>2.0698885511000005</v>
+        <v>2.3150761929</v>
       </c>
       <c r="I252" s="153"/>
       <c r="J252" s="153"/>
       <c r="K252" s="153"/>
       <c r="L252" s="153">
-        <v>-0.42341142870000015</v>
+        <v>-0.17822378690000074</v>
       </c>
       <c r="M252" s="153"/>
       <c r="N252" s="153"/>
@@ -17301,13 +17301,13 @@
       <c r="R252" s="153"/>
       <c r="S252" s="153"/>
       <c r="T252" s="153">
-        <v>1.6621707619</v>
+        <v>2.0383747157</v>
       </c>
       <c r="U252" s="153"/>
       <c r="V252" s="153"/>
       <c r="W252" s="153"/>
       <c r="X252" s="153">
-        <v>-0.51539923390726927</v>
+        <v>-0.13919528010726934</v>
       </c>
       <c r="Y252" s="153"/>
       <c r="Z252" s="153"/>
@@ -17325,13 +17325,13 @@
       <c r="F253" s="161"/>
       <c r="G253" s="161"/>
       <c r="H253" s="161">
-        <v>0.95097192956510446</v>
+        <v>1.0636188470545271</v>
       </c>
       <c r="I253" s="161"/>
       <c r="J253" s="161"/>
       <c r="K253" s="161"/>
       <c r="L253" s="161">
-        <v>0.29510126579164309</v>
+        <v>0.40774818328106577</v>
       </c>
       <c r="M253" s="161"/>
       <c r="N253" s="161"/>
@@ -17343,13 +17343,13 @@
       <c r="R253" s="161"/>
       <c r="S253" s="161"/>
       <c r="T253" s="161">
-        <v>0.76365354833753007</v>
+        <v>0.93649348199728377</v>
       </c>
       <c r="U253" s="161"/>
       <c r="V253" s="161"/>
       <c r="W253" s="161"/>
       <c r="X253" s="161">
-        <v>0.19083668308497803</v>
+        <v>0.36367661674473173</v>
       </c>
       <c r="Y253" s="161"/>
       <c r="Z253" s="161"/>
@@ -18791,13 +18791,13 @@
       <c r="F288" s="161"/>
       <c r="G288" s="161"/>
       <c r="H288" s="161">
-        <v>1.8064838481254295</v>
+        <v>1.8613704641777253</v>
       </c>
       <c r="I288" s="161"/>
       <c r="J288" s="161"/>
       <c r="K288" s="161"/>
       <c r="L288" s="161">
-        <v>-2.869563025044509</v>
+        <v>-2.8146764089922129</v>
       </c>
       <c r="M288" s="161"/>
       <c r="N288" s="161"/>
@@ -18809,13 +18809,13 @@
       <c r="R288" s="161"/>
       <c r="S288" s="161"/>
       <c r="T288" s="161">
-        <v>1.7840798697176326</v>
+        <v>1.84754257271448</v>
       </c>
       <c r="U288" s="161"/>
       <c r="V288" s="161"/>
       <c r="W288" s="161"/>
       <c r="X288" s="161">
-        <v>-2.4920429253544789</v>
+        <v>-2.4285802223576312</v>
       </c>
       <c r="Y288" s="161"/>
       <c r="Z288" s="161"/>
@@ -19367,13 +19367,13 @@
       <c r="F304" s="158"/>
       <c r="G304" s="158"/>
       <c r="H304" s="158">
-        <v>45795.962207483935</v>
+        <v>45808.257779179505</v>
       </c>
       <c r="I304" s="158"/>
       <c r="J304" s="158"/>
       <c r="K304" s="158"/>
       <c r="L304" s="158">
-        <v>-60060.35514377636</v>
+        <v>-60048.059572080783</v>
       </c>
       <c r="M304" s="158"/>
       <c r="N304" s="158"/>
@@ -19385,13 +19385,13 @@
       <c r="R304" s="158"/>
       <c r="S304" s="158"/>
       <c r="T304" s="158">
-        <v>26361.7687565456</v>
+        <v>26421.26480797266</v>
       </c>
       <c r="U304" s="158"/>
       <c r="V304" s="158"/>
       <c r="W304" s="158"/>
       <c r="X304" s="158">
-        <v>-83407.102171031773</v>
+        <v>-83347.606119604709</v>
       </c>
       <c r="Y304" s="158"/>
       <c r="Z304" s="158"/>
@@ -19409,13 +19409,13 @@
       <c r="F305" s="158"/>
       <c r="G305" s="158"/>
       <c r="H305" s="158">
-        <v>2612.9444150695517</v>
+        <v>2615.6935983035346</v>
       </c>
       <c r="I305" s="158"/>
       <c r="J305" s="158"/>
       <c r="K305" s="158"/>
       <c r="L305" s="158">
-        <v>-606.76602009532792</v>
+        <v>-604.016836861345</v>
       </c>
       <c r="M305" s="158"/>
       <c r="N305" s="158"/>
@@ -19427,13 +19427,13 @@
       <c r="R305" s="158"/>
       <c r="S305" s="158"/>
       <c r="T305" s="158">
-        <v>1236.8453781675969</v>
+        <v>1242.2701117771451</v>
       </c>
       <c r="U305" s="158"/>
       <c r="V305" s="158"/>
       <c r="W305" s="158"/>
       <c r="X305" s="158">
-        <v>-2056.0994272824664</v>
+        <v>-2050.6746936729182</v>
       </c>
       <c r="Y305" s="158"/>
       <c r="Z305" s="158"/>
@@ -19451,13 +19451,13 @@
       <c r="F306" s="160"/>
       <c r="G306" s="160"/>
       <c r="H306" s="160">
-        <v>48408.9066225535</v>
+        <v>48423.951377483048</v>
       </c>
       <c r="I306" s="160"/>
       <c r="J306" s="160"/>
       <c r="K306" s="160"/>
       <c r="L306" s="160">
-        <v>-60667.121163871678</v>
+        <v>-60652.076408942128</v>
       </c>
       <c r="M306" s="160"/>
       <c r="N306" s="160"/>
@@ -19469,13 +19469,13 @@
       <c r="R306" s="160"/>
       <c r="S306" s="160"/>
       <c r="T306" s="160">
-        <v>27598.614134713222</v>
+        <v>27663.534919749804</v>
       </c>
       <c r="U306" s="160"/>
       <c r="V306" s="160"/>
       <c r="W306" s="160"/>
       <c r="X306" s="160">
-        <v>-85463.201598314234</v>
+        <v>-85398.280813277655</v>
       </c>
       <c r="Y306" s="160"/>
       <c r="Z306" s="160"/>
@@ -20917,13 +20917,13 @@
       <c r="F341" s="160"/>
       <c r="G341" s="160"/>
       <c r="H341" s="160">
-        <v>49098.042079759885</v>
+        <v>49113.086834689464</v>
       </c>
       <c r="I341" s="160"/>
       <c r="J341" s="160"/>
       <c r="K341" s="160"/>
       <c r="L341" s="160">
-        <v>-89912.9715340727</v>
+        <v>-89897.926779143134</v>
       </c>
       <c r="M341" s="160"/>
       <c r="N341" s="160"/>
@@ -20935,13 +20935,13 @@
       <c r="R341" s="160"/>
       <c r="S341" s="160"/>
       <c r="T341" s="160">
-        <v>29032.82966600102</v>
+        <v>29097.750451037628</v>
       </c>
       <c r="U341" s="160"/>
       <c r="V341" s="160"/>
       <c r="W341" s="160"/>
       <c r="X341" s="160">
-        <v>-114239.42736004019</v>
+        <v>-114174.50657500359</v>
       </c>
       <c r="Y341" s="160"/>
       <c r="Z341" s="160"/>
@@ -21539,13 +21539,13 @@
       <c r="F358" s="153"/>
       <c r="G358" s="153"/>
       <c r="H358" s="153">
-        <v>0.1978715415</v>
+        <v>0.1922796539</v>
       </c>
       <c r="I358" s="153"/>
       <c r="J358" s="153"/>
       <c r="K358" s="153"/>
       <c r="L358" s="153">
-        <v>-2.2862478415000003</v>
+        <v>-2.2918397291000003</v>
       </c>
       <c r="M358" s="153"/>
       <c r="N358" s="153"/>
@@ -21557,13 +21557,13 @@
       <c r="R358" s="153"/>
       <c r="S358" s="153"/>
       <c r="T358" s="153">
-        <v>0.1511573229</v>
+        <v>0.1678268238</v>
       </c>
       <c r="U358" s="153"/>
       <c r="V358" s="153"/>
       <c r="W358" s="153"/>
       <c r="X358" s="153">
-        <v>-2.0099084662999998</v>
+        <v>-1.9932389653999998</v>
       </c>
       <c r="Y358" s="153"/>
       <c r="Z358" s="153"/>
@@ -21581,13 +21581,13 @@
       <c r="F359" s="161"/>
       <c r="G359" s="161"/>
       <c r="H359" s="161">
-        <v>0.09090841220715834</v>
+        <v>0.088339323094579161</v>
       </c>
       <c r="I359" s="161"/>
       <c r="J359" s="161"/>
       <c r="K359" s="161"/>
       <c r="L359" s="161">
-        <v>0.030856011398227974</v>
+        <v>0.028286922285648795</v>
       </c>
       <c r="M359" s="161"/>
       <c r="N359" s="161"/>
@@ -21599,13 +21599,13 @@
       <c r="R359" s="161"/>
       <c r="S359" s="161"/>
       <c r="T359" s="161">
-        <v>0.069446430316123839</v>
+        <v>0.0771049235366095</v>
       </c>
       <c r="U359" s="161"/>
       <c r="V359" s="161"/>
       <c r="W359" s="161"/>
       <c r="X359" s="161">
-        <v>0.016645201238540588</v>
+        <v>0.024303694459026248</v>
       </c>
       <c r="Y359" s="161"/>
       <c r="Z359" s="161"/>
@@ -23047,13 +23047,13 @@
       <c r="F394" s="161"/>
       <c r="G394" s="161"/>
       <c r="H394" s="161">
-        <v>0.14617871372265667</v>
+        <v>0.14363286112490342</v>
       </c>
       <c r="I394" s="161"/>
       <c r="J394" s="161"/>
       <c r="K394" s="161"/>
       <c r="L394" s="161">
-        <v>-0.96226867501287527</v>
+        <v>-0.96481452761062858</v>
       </c>
       <c r="M394" s="161"/>
       <c r="N394" s="161"/>
@@ -23065,13 +23065,13 @@
       <c r="R394" s="161"/>
       <c r="S394" s="161"/>
       <c r="T394" s="161">
-        <v>0.21237297437734035</v>
+        <v>0.21893204085535192</v>
       </c>
       <c r="U394" s="161"/>
       <c r="V394" s="161"/>
       <c r="W394" s="161"/>
       <c r="X394" s="161">
-        <v>-0.89767578823298577</v>
+        <v>-0.89111672175497425</v>
       </c>
       <c r="Y394" s="161"/>
       <c r="Z394" s="161"/>
@@ -25577,16 +25577,16 @@
         <v>1141.5356260585909</v>
       </c>
       <c r="F464" s="2">
-        <v>-65.2926226744237</v>
+        <v>-65.4712264535741</v>
       </c>
       <c r="G464" s="2">
-        <v>-55.9003593069075</v>
+        <v>-54.5934007592003</v>
       </c>
       <c r="H464" s="2">
-        <v>-55.1129366734636</v>
+        <v>-52.4549844144693</v>
       </c>
       <c r="I464" s="2">
-        <v>-54.9396607874432</v>
+        <v>-51.279658446457894</v>
       </c>
     </row>
     <row r="479" ht="14.25" customHeight="1">
@@ -25664,7 +25664,7 @@
       <c r="K481" s="83"/>
       <c r="L481" s="83"/>
       <c r="M481" s="83">
-        <v>72.788947137546614</v>
+        <v>72.610343358396108</v>
       </c>
       <c r="N481" s="83"/>
       <c r="O481" s="83"/>
@@ -25672,7 +25672,7 @@
       <c r="Q481" s="83"/>
       <c r="R481" s="83"/>
       <c r="S481" s="86">
-        <v>-94.518904583016067</v>
+        <v>-94.532353662771371</v>
       </c>
       <c r="T481" s="86"/>
       <c r="U481" s="86"/>
@@ -25763,7 +25763,7 @@
       <c r="K484" s="83"/>
       <c r="L484" s="83"/>
       <c r="M484" s="83">
-        <v>22.843482734371641</v>
+        <v>22.664878955221134</v>
       </c>
       <c r="N484" s="83"/>
       <c r="O484" s="83"/>
@@ -25771,7 +25771,7 @@
       <c r="Q484" s="83"/>
       <c r="R484" s="83"/>
       <c r="S484" s="86">
-        <v>14.217413671858203</v>
+        <v>13.32439477610567</v>
       </c>
       <c r="T484" s="86"/>
       <c r="U484" s="86"/>
@@ -25829,7 +25829,7 @@
       <c r="K486" s="83"/>
       <c r="L486" s="83"/>
       <c r="M486" s="83">
-        <v>-65.292622674423711</v>
+        <v>-65.471226453574218</v>
       </c>
       <c r="N486" s="83"/>
       <c r="O486" s="83"/>
@@ -25837,7 +25837,7 @@
       <c r="Q486" s="83"/>
       <c r="R486" s="83"/>
       <c r="S486" s="86">
-        <v>-105.65793957317364</v>
+        <v>-105.67341650377593</v>
       </c>
       <c r="T486" s="86"/>
       <c r="U486" s="86"/>
@@ -25969,7 +25969,7 @@
       <c r="Q490" s="83"/>
       <c r="R490" s="83"/>
       <c r="S490" s="86">
-        <v>-94.518904583016067</v>
+        <v>-94.532353662771371</v>
       </c>
       <c r="T490" s="86"/>
       <c r="U490" s="86"/>
@@ -26023,7 +26023,7 @@
       <c r="K492" s="83"/>
       <c r="L492" s="83"/>
       <c r="M492" s="83">
-        <v>-184.8664790477693</v>
+        <v>-184.90155618637721</v>
       </c>
       <c r="N492" s="83"/>
       <c r="O492" s="83"/>
@@ -26031,7 +26031,7 @@
       <c r="Q492" s="83"/>
       <c r="R492" s="83"/>
       <c r="S492" s="86">
-        <v>-418.73530870305052</v>
+        <v>-418.79578652823659</v>
       </c>
       <c r="T492" s="86"/>
       <c r="U492" s="86"/>
@@ -26056,7 +26056,7 @@
       <c r="K493" s="83"/>
       <c r="L493" s="83"/>
       <c r="M493" s="83">
-        <v>-756.426143626655</v>
+        <v>-756.5696702671969</v>
       </c>
       <c r="N493" s="83"/>
       <c r="O493" s="83"/>
@@ -26064,7 +26064,7 @@
       <c r="Q493" s="83"/>
       <c r="R493" s="83"/>
       <c r="S493" s="86">
-        <v>-419.16714920955906</v>
+        <v>-419.2277089735008</v>
       </c>
       <c r="T493" s="86"/>
       <c r="U493" s="86"/>
@@ -26170,7 +26170,7 @@
       <c r="K497" s="83"/>
       <c r="L497" s="83"/>
       <c r="M497" s="83">
-        <v>265.61927085571261</v>
+        <v>273.06558022424889</v>
       </c>
       <c r="N497" s="83"/>
       <c r="O497" s="83"/>
@@ -26257,7 +26257,7 @@
       <c r="K500" s="83"/>
       <c r="L500" s="83"/>
       <c r="M500" s="83">
-        <v>70.382396229797621</v>
+        <v>77.8287055983339</v>
       </c>
       <c r="N500" s="83"/>
       <c r="O500" s="83"/>
@@ -26315,7 +26315,7 @@
       <c r="K502" s="83"/>
       <c r="L502" s="83"/>
       <c r="M502" s="83">
-        <v>-231.24557944223807</v>
+        <v>-223.79927007370179</v>
       </c>
       <c r="N502" s="83"/>
       <c r="O502" s="83"/>
@@ -26487,7 +26487,7 @@
       <c r="K508" s="83"/>
       <c r="L508" s="83"/>
       <c r="M508" s="83">
-        <v>-733.58877145802387</v>
+        <v>-732.12634313159015</v>
       </c>
       <c r="N508" s="83"/>
       <c r="O508" s="83"/>
@@ -26516,7 +26516,7 @@
       <c r="K509" s="83"/>
       <c r="L509" s="83"/>
       <c r="M509" s="83">
-        <v>-3001.6568079842145</v>
+        <v>-2995.6729269421121</v>
       </c>
       <c r="N509" s="83"/>
       <c r="O509" s="83"/>
@@ -31031,13 +31031,13 @@
         <v>0.6048540154442329</v>
       </c>
       <c r="D8" s="5">
-        <v>468.27344305534217</v>
+        <v>486.95327222941927</v>
       </c>
       <c r="E8" s="18">
         <v>3.3556385250339638</v>
       </c>
       <c r="F8" s="5">
-        <v>569.43013752531328</v>
+        <v>591.24281219611953</v>
       </c>
       <c r="G8" s="18">
         <v>-18.964454123862705</v>
@@ -31055,7 +31055,7 @@
         <v>3.6330266156450466</v>
       </c>
       <c r="L8" s="5">
-        <v>5.874353023896921</v>
+        <v>5.8737311223078494</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
@@ -31066,13 +31066,13 @@
         <v>1.0441077098958058</v>
       </c>
       <c r="D9" s="5">
-        <v>351.25927174019915</v>
+        <v>365.04709042354835</v>
       </c>
       <c r="E9" s="18">
         <v>4.1229112336073612</v>
       </c>
       <c r="F9" s="5">
-        <v>424.54167130678906</v>
+        <v>440.6853534656172</v>
       </c>
       <c r="G9" s="18">
         <v>-6.7779948156505094</v>
@@ -31090,7 +31090,7 @@
         <v>3.7162467634607923</v>
       </c>
       <c r="L9" s="5">
-        <v>5.5444482105426527</v>
+        <v>5.5411012728666815</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
@@ -31101,13 +31101,13 @@
         <v>1.3761979559066682</v>
       </c>
       <c r="D10" s="5">
-        <v>233.46256126795805</v>
+        <v>242.47366500952805</v>
       </c>
       <c r="E10" s="18">
         <v>4.54204816834801</v>
       </c>
       <c r="F10" s="5">
-        <v>279.122835070389</v>
+        <v>289.65140514706405</v>
       </c>
       <c r="G10" s="18">
         <v>1.524724269002889</v>
@@ -31125,7 +31125,7 @@
         <v>3.7812889919690535</v>
       </c>
       <c r="L10" s="5">
-        <v>5.2123343179186845</v>
+        <v>5.2066479877186485</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -31136,13 +31136,13 @@
         <v>1.0971856475014412</v>
       </c>
       <c r="D11" s="5">
-        <v>114.78847494649239</v>
+        <v>119.1462972003761</v>
       </c>
       <c r="E11" s="18">
         <v>3.2674024830580892</v>
       </c>
       <c r="F11" s="5">
-        <v>133.10567519986506</v>
+        <v>138.09140740176957</v>
       </c>
       <c r="G11" s="18">
         <v>1.6927991508945754</v>
@@ -31160,7 +31160,7 @@
         <v>3.7366446220039551</v>
       </c>
       <c r="L11" s="5">
-        <v>4.8777489507845013</v>
+        <v>4.8701396869399325</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
@@ -31195,7 +31195,7 @@
         <v>3.5374571916319586</v>
       </c>
       <c r="L12" s="5">
-        <v>4.5541238999171449</v>
+        <v>4.5450451352843553</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
@@ -31206,13 +31206,13 @@
         <v>-0.86898845936118152</v>
       </c>
       <c r="D13" s="5">
-        <v>-71.243966332150364</v>
+        <v>-73.948966369147072</v>
       </c>
       <c r="E13" s="18">
         <v>-2.7613949898480303</v>
       </c>
       <c r="F13" s="5">
-        <v>-80.574059823532664</v>
+        <v>-83.596663990059255</v>
       </c>
       <c r="G13" s="18">
         <v>-0.789776657474845</v>
@@ -31230,7 +31230,7 @@
         <v>3.3756698248445023</v>
       </c>
       <c r="L13" s="5">
-        <v>4.3532783683369329</v>
+        <v>4.3432867366126464</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -31241,13 +31241,13 @@
         <v>-0.48111912697254244</v>
       </c>
       <c r="D14" s="5">
-        <v>-82.726987115066621</v>
+        <v>-86.712084986110725</v>
       </c>
       <c r="E14" s="18">
         <v>-3.0302358029182663</v>
       </c>
       <c r="F14" s="5">
-        <v>-89.345284951847631</v>
+        <v>-93.213890326165853</v>
       </c>
       <c r="G14" s="18">
         <v>0.18230985045243003</v>
@@ -31265,7 +31265,7 @@
         <v>3.4483417075074367</v>
       </c>
       <c r="L14" s="5">
-        <v>4.3209265525276166</v>
+        <v>4.3084845263129665</v>
       </c>
     </row>
     <row r="15" hidden="1" ht="14.25" customHeight="1">
@@ -31291,13 +31291,13 @@
         <v>-3.7715605622843715</v>
       </c>
       <c r="D16" s="5">
-        <v>-76.470925606337261</v>
+        <v>-79.043577675263066</v>
       </c>
       <c r="E16" s="18">
         <v>-9.3238441836033612</v>
       </c>
       <c r="F16" s="5">
-        <v>-99.374001099234476</v>
+        <v>-102.63073764166167</v>
       </c>
       <c r="G16" s="18">
         <v>-5.842035815889143</v>
@@ -31315,7 +31315,7 @@
         <v>2.8344602123667095</v>
       </c>
       <c r="L16" s="5">
-        <v>4.3385650496449371</v>
+        <v>4.3294090896351873</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -31326,13 +31326,13 @@
         <v>-1.1279825030050532</v>
       </c>
       <c r="D17" s="5">
-        <v>347.7293174430713</v>
+        <v>361.6225358433415</v>
       </c>
       <c r="E17" s="18">
         <v>-0.90249935086708366</v>
       </c>
       <c r="F17" s="5">
-        <v>386.63006451086051</v>
+        <v>401.57626450132381</v>
       </c>
       <c r="G17" s="18">
         <v>-2.9710114540948189</v>
@@ -31350,7 +31350,7 @@
         <v>3.3142696898230817</v>
       </c>
       <c r="L17" s="5">
-        <v>5.5344977076652038</v>
+        <v>5.5317588428607785</v>
       </c>
     </row>
     <row r="18" hidden="1" ht="14.25" customHeight="1">
@@ -31420,10 +31420,10 @@
         <v>4407.6907353066917</v>
       </c>
       <c r="D22" s="49">
-        <v>-231.245579442238</v>
+        <v>-223.79927007370162</v>
       </c>
       <c r="E22" s="49">
-        <v>-4638.9363147489294</v>
+        <v>-4631.4900053803931</v>
       </c>
       <c r="F22" s="49">
         <v>-1615.5575863538329</v>
@@ -31435,7 +31435,7 @@
       <c r="I22" s="49"/>
       <c r="J22" s="49"/>
       <c r="K22" s="49">
-        <v>-2517.4556290896021</v>
+        <v>-2510.0093197210658</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -31446,10 +31446,10 @@
         <v>8326.0272920950974</v>
       </c>
       <c r="D23" s="49">
-        <v>-454.48319091922912</v>
+        <v>-439.79001070509332</v>
       </c>
       <c r="E23" s="49">
-        <v>-8780.5104830143264</v>
+        <v>-8765.8173028001911</v>
       </c>
       <c r="F23" s="49">
         <v>-3231.1151727076658</v>
@@ -31461,7 +31461,7 @@
       <c r="I23" s="49"/>
       <c r="J23" s="49"/>
       <c r="K23" s="49">
-        <v>-4537.5491116956719</v>
+        <v>-4522.8559314815366</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
@@ -31472,10 +31472,10 @@
         <v>671.76678338114948</v>
       </c>
       <c r="D24" s="49">
-        <v>-3001.6568079842145</v>
+        <v>-2995.6729269421121</v>
       </c>
       <c r="E24" s="49">
-        <v>-3673.4235913653642</v>
+        <v>-3667.4397103232614</v>
       </c>
       <c r="F24" s="49">
         <v>-1615.5575863538329</v>
@@ -31490,10 +31490,10 @@
         <v>2.0000000000000511</v>
       </c>
       <c r="J24" s="49">
-        <v>897.51272338356739</v>
+        <v>896.05029505713367</v>
       </c>
       <c r="K24" s="49">
-        <v>-2517.4556290896044</v>
+        <v>-2510.0093197210681</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
@@ -31504,10 +31504,10 @@
         <v>950.16809249182882</v>
       </c>
       <c r="D25" s="49">
-        <v>-5996.8783840540136</v>
+        <v>-5985.0708914855395</v>
       </c>
       <c r="E25" s="49">
-        <v>-6947.0464765458428</v>
+        <v>-6935.2389839773678</v>
       </c>
       <c r="F25" s="49">
         <v>-3231.1151727076658</v>
@@ -31522,10 +31522,10 @@
         <v>4.0000000000001021</v>
       </c>
       <c r="J25" s="49">
-        <v>1697.4640064684841</v>
+        <v>1694.5783188228249</v>
       </c>
       <c r="K25" s="49">
-        <v>-4537.5491116956719</v>
+        <v>-4522.8559314815384</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
@@ -31673,31 +31673,31 @@
         <v>154</v>
       </c>
       <c r="C36" s="49">
-        <v>-39.943078732896623</v>
+        <v>-29.738256809098015</v>
       </c>
       <c r="D36" s="49">
-        <v>-66.497056679823928</v>
+        <v>-58.302023112503385</v>
       </c>
       <c r="E36" s="49">
-        <v>-231.245579442238</v>
+        <v>-223.79927007370162</v>
       </c>
       <c r="F36" s="49">
-        <v>-496.68885346516248</v>
+        <v>-490.44781352798651</v>
       </c>
       <c r="G36" s="49">
-        <v>-771.11743202701746</v>
+        <v>-766.45356248597784</v>
       </c>
       <c r="H36" s="49">
-        <v>-1043.517117722447</v>
+        <v>-1040.7719938668884</v>
       </c>
       <c r="I36" s="49">
-        <v>-1314.1072162096823</v>
+        <v>-1313.5971389231472</v>
       </c>
       <c r="J36" s="49">
-        <v>-1035.3542544540073</v>
+        <v>-1033.10786571311</v>
       </c>
       <c r="K36" s="50">
-        <v>114.78847494649239</v>
+        <v>119.1462972003761</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -32240,28 +32240,28 @@
         <v>25.3701895355351</v>
       </c>
       <c r="H52" s="49">
-        <v>23.9501805327689</v>
+        <v>23.7334629925411</v>
       </c>
       <c r="I52" s="49">
-        <v>23.468577069242603</v>
+        <v>23.5066908303199</v>
       </c>
       <c r="J52" s="49">
-        <v>23.0259294553914</v>
+        <v>23.266306149136998</v>
       </c>
       <c r="K52" s="49">
-        <v>22.5843635821507</v>
+        <v>23.0199105548528</v>
       </c>
       <c r="L52" s="49">
-        <v>22.1802641755488</v>
+        <v>22.811299056808398</v>
       </c>
       <c r="M52" s="49">
-        <v>21.8245350392199</v>
+        <v>22.5711842379646</v>
       </c>
       <c r="N52" s="49">
-        <v>21.7928975726436</v>
+        <v>22.7346591537199</v>
       </c>
       <c r="O52" s="49">
-        <v>20.6425524922044</v>
+        <v>21.6120939713776</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -32312,28 +32312,28 @@
         <v>-23.3557986562562</v>
       </c>
       <c r="H54" s="49">
-        <v>-21.8956281267881</v>
+        <v>-22.112345667015802</v>
       </c>
       <c r="I54" s="49">
-        <v>-20.0411958913794</v>
+        <v>-20.0030821303021</v>
       </c>
       <c r="J54" s="49">
-        <v>-18.4775837252878</v>
+        <v>-18.237207031542198</v>
       </c>
       <c r="K54" s="49">
-        <v>-18.5628732390847</v>
+        <v>-18.127326266382703</v>
       </c>
       <c r="L54" s="49">
-        <v>-18.859902342534998</v>
+        <v>-18.2288674612754</v>
       </c>
       <c r="M54" s="49">
-        <v>-18.726914150082298</v>
+        <v>-17.980264951337602</v>
       </c>
       <c r="N54" s="49">
-        <v>-17.9688835210771</v>
+        <v>-17.0271219400008</v>
       </c>
       <c r="O54" s="49">
-        <v>-18.4171390023042</v>
+        <v>-17.4475975231309</v>
       </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
@@ -32420,28 +32420,28 @@
         <v>-315.355798656256</v>
       </c>
       <c r="H57" s="49">
-        <v>-313.895628126788</v>
+        <v>-314.112345667016</v>
       </c>
       <c r="I57" s="49">
-        <v>-312.04119589137895</v>
+        <v>-312.003082130302</v>
       </c>
       <c r="J57" s="49">
-        <v>-310.477583725288</v>
+        <v>-310.237207031542</v>
       </c>
       <c r="K57" s="49">
-        <v>-310.56287323908504</v>
+        <v>-310.127326266383</v>
       </c>
       <c r="L57" s="49">
-        <v>-310.85990234253495</v>
+        <v>-310.228867461275</v>
       </c>
       <c r="M57" s="49">
-        <v>-310.726914150082</v>
+        <v>-309.98026495133803</v>
       </c>
       <c r="N57" s="49">
-        <v>-309.968883521077</v>
+        <v>-309.027121940001</v>
       </c>
       <c r="O57" s="49">
-        <v>-310.417139002304</v>
+        <v>-309.447597523131</v>
       </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
@@ -32456,28 +32456,28 @@
         <v>-61.9347424387961</v>
       </c>
       <c r="H58" s="49">
-        <v>-61.6479702086844</v>
+        <v>-61.690532752621</v>
       </c>
       <c r="I58" s="49">
-        <v>-61.2837664002888</v>
+        <v>-61.276280994960096</v>
       </c>
       <c r="J58" s="49">
-        <v>-60.976678605506905</v>
+        <v>-60.9294694890775</v>
       </c>
       <c r="K58" s="49">
-        <v>-60.993429158667</v>
+        <v>-60.9078893027669</v>
       </c>
       <c r="L58" s="49">
-        <v>-61.0517646042095</v>
+        <v>-60.9278316275296</v>
       </c>
       <c r="M58" s="49">
-        <v>-61.0256462024485</v>
+        <v>-60.879006990442804</v>
       </c>
       <c r="N58" s="49">
-        <v>-60.8767717185538</v>
+        <v>-60.6918131377658</v>
       </c>
       <c r="O58" s="49">
-        <v>-60.964807479731704</v>
+        <v>-60.7743930270652</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -32492,28 +32492,28 @@
         <v>-253.42105621745998</v>
       </c>
       <c r="H59" s="49">
-        <v>-252.247657918104</v>
+        <v>-252.42181291439502</v>
       </c>
       <c r="I59" s="49">
-        <v>-250.757429491091</v>
+        <v>-250.726801135342</v>
       </c>
       <c r="J59" s="49">
-        <v>-249.500905119781</v>
+        <v>-249.30773754246502</v>
       </c>
       <c r="K59" s="49">
-        <v>-249.569444080418</v>
+        <v>-249.219436963616</v>
       </c>
       <c r="L59" s="49">
-        <v>-249.80813773832603</v>
+        <v>-249.301035833746</v>
       </c>
       <c r="M59" s="49">
-        <v>-249.70126794763402</v>
+        <v>-249.101257960895</v>
       </c>
       <c r="N59" s="49">
-        <v>-249.092111802523</v>
+        <v>-248.335308802235</v>
       </c>
       <c r="O59" s="49">
-        <v>-249.452331522572</v>
+        <v>-248.673204496066</v>
       </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
@@ -32530,28 +32530,28 @@
         <v>-68880.3156865193</v>
       </c>
       <c r="H60" s="49">
-        <v>-69132.563344437411</v>
+        <v>-69132.737499433613</v>
       </c>
       <c r="I60" s="49">
-        <v>-69383.320773927</v>
+        <v>-69383.4643005676</v>
       </c>
       <c r="J60" s="49">
-        <v>-69632.8216790482</v>
+        <v>-69632.772038111492</v>
       </c>
       <c r="K60" s="49">
-        <v>-69882.391123128691</v>
+        <v>-69881.99147507509</v>
       </c>
       <c r="L60" s="49">
-        <v>-70132.19926086851</v>
+        <v>-70131.292510910309</v>
       </c>
       <c r="M60" s="49">
-        <v>-70381.9005288147</v>
+        <v>-70380.3937688698</v>
       </c>
       <c r="N60" s="49">
-        <v>-70630.992640618613</v>
+        <v>-70628.729077673488</v>
       </c>
       <c r="O60" s="49">
-        <v>-70880.4449721426</v>
+        <v>-70877.402282170908</v>
       </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
@@ -32619,10 +32619,10 @@
         <v>0</v>
       </c>
       <c r="F65" s="49">
-        <v>265.61927085571261</v>
+        <v>273.06558022424889</v>
       </c>
       <c r="G65" s="49">
-        <v>401.8357614472967</v>
+        <v>402.34583873383275</v>
       </c>
       <c r="H65" s="49">
         <f>G65-F65</f>
@@ -32733,10 +32733,10 @@
         <f>IF(OR(C68="",D68=""),"",D68-C68)</f>
       </c>
       <c r="F68" s="49">
-        <v>70.382396229797664</v>
+        <v>77.828705598333869</v>
       </c>
       <c r="G68" s="49">
-        <v>178.22665179301202</v>
+        <v>178.7367290795485</v>
       </c>
       <c r="H68" s="49">
         <f>IF(OR(F68="",G68=""),"",G68-F68)</f>
@@ -33136,10 +33136,10 @@
         <v>0</v>
       </c>
       <c r="F82" s="49">
-        <v>265.61927085571261</v>
+        <v>273.06558022424889</v>
       </c>
       <c r="G82" s="49">
-        <v>369.4092912916143</v>
+        <v>372.15441514717349</v>
       </c>
       <c r="H82" s="49">
         <f>G82-F82</f>
@@ -33250,10 +33250,10 @@
         <f>IF(OR(C85="",D85=""),"",D85-C85)</f>
       </c>
       <c r="F85" s="49">
-        <v>70.382396229797664</v>
+        <v>77.828705598333869</v>
       </c>
       <c r="G85" s="49">
-        <v>152.60551964121902</v>
+        <v>155.350643496778</v>
       </c>
       <c r="H85" s="49">
         <f>IF(OR(F85="",G85=""),"",G85-F85)</f>
@@ -33653,10 +33653,10 @@
         <v>0</v>
       </c>
       <c r="F99" s="49">
-        <v>265.61927085571261</v>
+        <v>273.06558022424889</v>
       </c>
       <c r="G99" s="49">
-        <v>335.83257986190415</v>
+        <v>340.49644940294382</v>
       </c>
       <c r="H99" s="49">
         <f>G99-F99</f>
@@ -33767,10 +33767,10 @@
         <f>IF(OR(C102="",D102=""),"",D102-C102)</f>
       </c>
       <c r="F102" s="49">
-        <v>70.382396229797664</v>
+        <v>77.828705598333869</v>
       </c>
       <c r="G102" s="49">
-        <v>126.1033407939134</v>
+        <v>130.76721033495304</v>
       </c>
       <c r="H102" s="49">
         <f>IF(OR(F102="",G102=""),"",G102-F102)</f>
@@ -34170,10 +34170,10 @@
         <v>0</v>
       </c>
       <c r="F116" s="49">
-        <v>265.61927085571261</v>
+        <v>273.06558022424889</v>
       </c>
       <c r="G116" s="49">
-        <v>301.26853734515061</v>
+        <v>307.50957728232663</v>
       </c>
       <c r="H116" s="49">
         <f>G116-F116</f>
@@ -34284,10 +34284,10 @@
         <f>IF(OR(C119="",D119=""),"",D119-C119)</f>
       </c>
       <c r="F119" s="49">
-        <v>70.382396229797664</v>
+        <v>77.828705598333869</v>
       </c>
       <c r="G119" s="49">
-        <v>98.7056325062723</v>
+        <v>104.94667244344836</v>
       </c>
       <c r="H119" s="49">
         <f>IF(OR(F119="",G119=""),"",G119-F119)</f>
@@ -34687,10 +34687,10 @@
         <v>0</v>
       </c>
       <c r="F133" s="49">
-        <v>265.61927085571261</v>
+        <v>273.06558022424889</v>
       </c>
       <c r="G133" s="49">
-        <v>222.36106045051551</v>
+        <v>230.55609401783613</v>
       </c>
       <c r="H133" s="49">
         <f>G133-F133</f>
@@ -34801,10 +34801,10 @@
         <f>IF(OR(C136="",D136=""),"",D136-C136)</f>
       </c>
       <c r="F136" s="49">
-        <v>70.382396229797664</v>
+        <v>77.828705598333869</v>
       </c>
       <c r="G136" s="49">
-        <v>41.013018214660931</v>
+        <v>49.208051781981446</v>
       </c>
       <c r="H136" s="49">
         <f>IF(OR(F136="",G136=""),"",G136-F136)</f>
@@ -35204,10 +35204,10 @@
         <v>0</v>
       </c>
       <c r="F150" s="49">
-        <v>265.61927085571261</v>
+        <v>273.06558022424889</v>
       </c>
       <c r="G150" s="49">
-        <v>182.18121835569406</v>
+        <v>192.3860402794929</v>
       </c>
       <c r="H150" s="49">
         <f>G150-F150</f>
@@ -35318,10 +35318,10 @@
         <f>IF(OR(C153="",D153=""),"",D153-C153)</f>
       </c>
       <c r="F153" s="49">
-        <v>70.382396229797664</v>
+        <v>77.828705598333869</v>
       </c>
       <c r="G153" s="49">
-        <v>12.356141507791993</v>
+        <v>22.560963431590668</v>
       </c>
       <c r="H153" s="49">
         <f>IF(OR(F153="",G153=""),"",G153-F153)</f>
@@ -37226,31 +37226,31 @@
         <v>10.4777549623546</v>
       </c>
       <c r="M28" s="168">
-        <v>38.1036509417304</v>
+        <v>38.1036509417303</v>
       </c>
       <c r="N28" s="168">
         <v>32.0730613627913</v>
       </c>
       <c r="O28" s="167">
-        <v>118.8026628039172</v>
+        <v>118.80266280391689</v>
       </c>
       <c r="P28" s="167">
-        <v>-10.533788030045466</v>
+        <v>-10.533788030045232</v>
       </c>
       <c r="Q28" s="167">
-        <v>1.74712941973342</v>
+        <v>1.74712941973343</v>
       </c>
       <c r="R28" s="167">
         <v>0</v>
       </c>
       <c r="S28" s="167">
-        <v>-0.8287669139606002</v>
+        <v>-0.82876691396059021</v>
       </c>
       <c r="T28" s="168">
         <v>-1508.9325353838015</v>
       </c>
       <c r="U28" s="168">
-        <v>1.822738998292005</v>
+        <v>1.8227389982919047</v>
       </c>
       <c r="V28" s="168">
         <v>-1507.1097963855095</v>
@@ -37262,7 +37262,7 @@
         <v>-0.19180153977603759</v>
       </c>
       <c r="Y28" s="169">
-        <v>0.047836334661983157</v>
+        <v>0.047836334661980652</v>
       </c>
       <c r="Z28" s="169">
         <v>0</v>
@@ -37271,7 +37271,7 @@
         <v>0.7136137967076055</v>
       </c>
       <c r="AB28" s="169">
-        <v>-0.47435920006833548</v>
+        <v>-0.47435920006832705</v>
       </c>
     </row>
     <row r="29">
@@ -37321,13 +37321,13 @@
         <v>-16.224349537640233</v>
       </c>
       <c r="Q29" s="167">
-        <v>4.45578905757086</v>
+        <v>4.45578905757172</v>
       </c>
       <c r="R29" s="167">
         <v>0</v>
       </c>
       <c r="S29" s="167">
-        <v>1.8798927238776004</v>
+        <v>1.8798927238784602</v>
       </c>
       <c r="T29" s="168">
         <v>-1904.5171885613474</v>
@@ -37354,7 +37354,7 @@
         <v>0.46300832925036811</v>
       </c>
       <c r="AB29" s="169">
-        <v>0.42189894979060161</v>
+        <v>0.42189894979071313</v>
       </c>
     </row>
     <row r="30">
@@ -37392,31 +37392,31 @@
         <v>7.61396303901437</v>
       </c>
       <c r="M30" s="176">
-        <v>91.766658768599</v>
+        <v>91.7666587685989</v>
       </c>
       <c r="N30" s="176">
         <v>82.4412730977237</v>
       </c>
       <c r="O30" s="175">
-        <v>111.31154981051935</v>
+        <v>111.31154981051922</v>
       </c>
       <c r="P30" s="175">
-        <v>-13.861496054060705</v>
+        <v>-13.861496054060611</v>
       </c>
       <c r="Q30" s="175">
-        <v>3.33109058053062</v>
+        <v>3.33109058053116</v>
       </c>
       <c r="R30" s="175">
         <v>0</v>
       </c>
       <c r="S30" s="175">
-        <v>0.75519424683709024</v>
+        <v>0.75519424683763026</v>
       </c>
       <c r="T30" s="176">
         <v>-3413.4497239451484</v>
       </c>
       <c r="U30" s="176">
-        <v>-1.4905621723822031</v>
+        <v>-1.4905621723823086</v>
       </c>
       <c r="V30" s="176">
         <v>-3414.9402861175308</v>
@@ -37428,7 +37428,7 @@
         <v>-0.50471144426373316</v>
       </c>
       <c r="Y30" s="177">
-        <v>-0.016242960050892125</v>
+        <v>-0.016242960050893294</v>
       </c>
       <c r="Z30" s="177">
         <v>0</v>
@@ -37437,7 +37437,7 @@
         <v>0.60589715929521781</v>
       </c>
       <c r="AB30" s="177">
-        <v>0.22671081094312148</v>
+        <v>0.22671081094324685</v>
       </c>
     </row>
     <row r="31">
@@ -38799,13 +38799,13 @@
         <v>-8.1676201945729865</v>
       </c>
       <c r="Q47" s="175">
-        <v>2.1133528313297</v>
+        <v>2.11335283132976</v>
       </c>
       <c r="R47" s="175">
         <v>12.894126304230408</v>
       </c>
       <c r="S47" s="175">
-        <v>0.6000775676855401</v>
+        <v>0.6000775676856</v>
       </c>
       <c r="T47" s="176">
         <v>-82570.874365356038</v>
@@ -38832,7 +38832,7 @@
         <v>-0.45130142737196377</v>
       </c>
       <c r="AB47" s="177">
-        <v>0.28394575614142831</v>
+        <v>0.28394575614144862</v>
       </c>
     </row>
     <row r="48">
@@ -40451,19 +40451,19 @@
         <v>9020.05634563938</v>
       </c>
       <c r="D19" s="166">
-        <v>3074.39877694932</v>
+        <v>3077.63347475744</v>
       </c>
       <c r="E19" s="166">
-        <v>-5945.65756869006</v>
+        <v>-5942.42287088194</v>
       </c>
       <c r="F19" s="166">
         <v>9225.2232883542</v>
       </c>
       <c r="G19" s="166">
-        <v>1455.27623778888</v>
+        <v>1461.6589967478099</v>
       </c>
       <c r="H19" s="166">
-        <v>-7769.9470505653189</v>
+        <v>-7763.56429160639</v>
       </c>
     </row>
     <row r="20">
@@ -40474,19 +40474,19 @@
         <v>3219.71043516488</v>
       </c>
       <c r="D20" s="166">
-        <v>2612.94441506955</v>
+        <v>2615.69359830353</v>
       </c>
       <c r="E20" s="166">
-        <v>-606.76602009533019</v>
+        <v>-604.01683686135016</v>
       </c>
       <c r="F20" s="166">
         <v>3292.9448054500704</v>
       </c>
       <c r="G20" s="166">
-        <v>1236.8453781675999</v>
+        <v>1242.27011177715</v>
       </c>
       <c r="H20" s="166">
-        <v>-2056.09942728247</v>
+        <v>-2050.67469367292</v>
       </c>
     </row>
     <row r="21">
@@ -40497,19 +40497,19 @@
         <v>12239.7667808043</v>
       </c>
       <c r="D21" s="181">
-        <v>5687.3431920188705</v>
+        <v>5693.32707306097</v>
       </c>
       <c r="E21" s="181">
-        <v>-6552.42358878543</v>
+        <v>-6546.4397077433305</v>
       </c>
       <c r="F21" s="181">
         <v>12518.1680938043</v>
       </c>
       <c r="G21" s="181">
-        <v>2692.12161595648</v>
+        <v>2703.92910852496</v>
       </c>
       <c r="H21" s="181">
-        <v>-9826.04647784782</v>
+        <v>-9814.23898527934</v>
       </c>
     </row>
     <row r="22">
@@ -41298,19 +41298,19 @@
         <v>103901.766780804</v>
       </c>
       <c r="D56" s="181">
-        <v>12588.4068950503</v>
+        <v>12594.390776092401</v>
       </c>
       <c r="E56" s="181">
-        <v>-91313.3598857537</v>
+        <v>-91307.3760047116</v>
       </c>
       <c r="F56" s="181">
         <v>104180.16809380401</v>
       </c>
       <c r="G56" s="181">
-        <v>9593.1853189879512</v>
+        <v>9604.99281155642</v>
       </c>
       <c r="H56" s="181">
-        <v>-94586.982774816046</v>
+        <v>-94575.175282247583</v>
       </c>
     </row>
     <row r="57"/>
@@ -41526,19 +41526,19 @@
         <v>12235.7667808042</v>
       </c>
       <c r="D68" s="181">
-        <v>-71628.551438283</v>
+        <v>-71622.567557240909</v>
       </c>
       <c r="E68" s="181">
-        <v>-83864.3182190872</v>
+        <v>-83858.3343380451</v>
       </c>
       <c r="F68" s="181">
         <v>12514.1680938043</v>
       </c>
       <c r="G68" s="181">
-        <v>-74623.7730143454</v>
+        <v>-74611.9655217769</v>
       </c>
       <c r="H68" s="181">
-        <v>-87137.9411081497</v>
+        <v>-87126.1336155812</v>
       </c>
     </row>
     <row r="69">
@@ -41635,19 +41635,19 @@
         <v>78107.665236501431</v>
       </c>
       <c r="D75" s="166">
-        <v>70382.396229797669</v>
+        <v>77828.705598333865</v>
       </c>
       <c r="E75" s="166">
-        <v>-7725.269006703762</v>
+        <v>-278.95963816756557</v>
       </c>
       <c r="F75" s="166">
         <v>70949.956660706361</v>
       </c>
       <c r="G75" s="166">
-        <v>33396.8854813406</v>
+        <v>40643.756326939627</v>
       </c>
       <c r="H75" s="166">
-        <v>-37553.071179365761</v>
+        <v>-30306.200333766734</v>
       </c>
     </row>
     <row r="76">
@@ -41658,19 +41658,19 @@
         <v>78107.665236501431</v>
       </c>
       <c r="D76" s="181">
-        <v>70382.396229797669</v>
+        <v>77828.705598333865</v>
       </c>
       <c r="E76" s="181">
-        <v>-7725.269006703762</v>
+        <v>-278.95963816756557</v>
       </c>
       <c r="F76" s="181">
         <v>70949.956660706361</v>
       </c>
       <c r="G76" s="181">
-        <v>33396.8854813406</v>
+        <v>40643.756326939627</v>
       </c>
       <c r="H76" s="181">
-        <v>-37553.071179365761</v>
+        <v>-30306.200333766734</v>
       </c>
     </row>
     <row r="77">
@@ -42459,19 +42459,19 @@
         <v>5155967.0767253377</v>
       </c>
       <c r="D111" s="181">
-        <v>265619.27085571259</v>
+        <v>273065.58022424887</v>
       </c>
       <c r="E111" s="181">
-        <v>-4890347.805869625</v>
+        <v>-4882901.4965010891</v>
       </c>
       <c r="F111" s="181">
         <v>4807899.2204189058</v>
       </c>
       <c r="G111" s="181">
-        <v>210370.08954861396</v>
+        <v>217616.96039421292</v>
       </c>
       <c r="H111" s="181">
-        <v>-4597529.130870292</v>
+        <v>-4590282.2600246929</v>
       </c>
     </row>
     <row r="112"/>
@@ -42687,19 +42687,19 @@
         <v>4407690.7353066914</v>
       </c>
       <c r="D123" s="181">
-        <v>-231245.579442238</v>
+        <v>-223799.27007370163</v>
       </c>
       <c r="E123" s="181">
-        <v>-4638936.31474893</v>
+        <v>-4631490.005380393</v>
       </c>
       <c r="F123" s="181">
         <v>3918336.5567884049</v>
       </c>
       <c r="G123" s="181">
-        <v>-223237.61147699109</v>
+        <v>-215990.7406313917</v>
       </c>
       <c r="H123" s="181">
-        <v>-4141574.1682653958</v>
+        <v>-4134327.2974197967</v>
       </c>
     </row>
     <row r="124">
@@ -42800,19 +42800,19 @@
         <v>2.4932999798000006</v>
       </c>
       <c r="D130" s="165">
-        <v>2.0698885511000005</v>
+        <v>2.3150761929</v>
       </c>
       <c r="E130" s="165">
-        <v>-0.42341142870000015</v>
+        <v>-0.17822378690000074</v>
       </c>
       <c r="F130" s="165">
         <v>2.1775699958072692</v>
       </c>
       <c r="G130" s="165">
-        <v>1.6621707619</v>
+        <v>2.0383747157</v>
       </c>
       <c r="H130" s="165">
-        <v>-0.51539923390726927</v>
+        <v>-0.13919528010726934</v>
       </c>
     </row>
     <row r="131">
@@ -42823,19 +42823,19 @@
         <v>0.65587066377346137</v>
       </c>
       <c r="D131" s="182">
-        <v>0.95097192956510446</v>
+        <v>1.0636188470545271</v>
       </c>
       <c r="E131" s="182">
-        <v>0.29510126579164309</v>
+        <v>0.40774818328106577</v>
       </c>
       <c r="F131" s="182">
         <v>0.572816865252552</v>
       </c>
       <c r="G131" s="182">
-        <v>0.76365354833753007</v>
+        <v>0.93649348199728377</v>
       </c>
       <c r="H131" s="182">
-        <v>0.19083668308497803</v>
+        <v>0.36367661674473173</v>
       </c>
     </row>
     <row r="132">
@@ -43624,19 +43624,19 @@
         <v>4.6760468731699385</v>
       </c>
       <c r="D166" s="182">
-        <v>1.8064838481254295</v>
+        <v>1.8613704641777253</v>
       </c>
       <c r="E166" s="182">
-        <v>-2.869563025044509</v>
+        <v>-2.8146764089922129</v>
       </c>
       <c r="F166" s="182">
         <v>4.2761227950721112</v>
       </c>
       <c r="G166" s="182">
-        <v>1.7840798697176326</v>
+        <v>1.84754257271448</v>
       </c>
       <c r="H166" s="182">
-        <v>-2.4920429253544789</v>
+        <v>-2.4285802223576312</v>
       </c>
     </row>
     <row r="167"/>
@@ -43914,19 +43914,19 @@
         <v>105856.3173512603</v>
       </c>
       <c r="D182" s="166">
-        <v>45795.962207483935</v>
+        <v>45808.257779179505</v>
       </c>
       <c r="E182" s="166">
-        <v>-60060.35514377636</v>
+        <v>-60048.059572080783</v>
       </c>
       <c r="F182" s="166">
         <v>109768.87092757737</v>
       </c>
       <c r="G182" s="166">
-        <v>26361.7687565456</v>
+        <v>26421.26480797266</v>
       </c>
       <c r="H182" s="166">
-        <v>-83407.102171031773</v>
+        <v>-83347.606119604709</v>
       </c>
     </row>
     <row r="183">
@@ -43937,19 +43937,19 @@
         <v>3219.7104351648795</v>
       </c>
       <c r="D183" s="166">
-        <v>2612.9444150695517</v>
+        <v>2615.6935983035346</v>
       </c>
       <c r="E183" s="166">
-        <v>-606.76602009532792</v>
+        <v>-604.016836861345</v>
       </c>
       <c r="F183" s="166">
         <v>3292.9448054500631</v>
       </c>
       <c r="G183" s="166">
-        <v>1236.8453781675969</v>
+        <v>1242.2701117771451</v>
       </c>
       <c r="H183" s="166">
-        <v>-2056.0994272824664</v>
+        <v>-2050.6746936729182</v>
       </c>
     </row>
     <row r="184">
@@ -43960,19 +43960,19 @@
         <v>109076.02778642517</v>
       </c>
       <c r="D184" s="181">
-        <v>48408.9066225535</v>
+        <v>48423.951377483048</v>
       </c>
       <c r="E184" s="181">
-        <v>-60667.121163871678</v>
+        <v>-60652.076408942128</v>
       </c>
       <c r="F184" s="181">
         <v>113061.81573302746</v>
       </c>
       <c r="G184" s="181">
-        <v>27598.614134713222</v>
+        <v>27663.534919749804</v>
       </c>
       <c r="H184" s="181">
-        <v>-85463.201598314234</v>
+        <v>-85398.280813277655</v>
       </c>
     </row>
     <row r="185">
@@ -44761,19 +44761,19 @@
         <v>139011.01361383259</v>
       </c>
       <c r="D219" s="181">
-        <v>49098.042079759885</v>
+        <v>49113.086834689464</v>
       </c>
       <c r="E219" s="181">
-        <v>-89912.9715340727</v>
+        <v>-89897.926779143134</v>
       </c>
       <c r="F219" s="181">
         <v>143272.25702604122</v>
       </c>
       <c r="G219" s="181">
-        <v>29032.82966600102</v>
+        <v>29097.750451037628</v>
       </c>
       <c r="H219" s="181">
-        <v>-114239.42736004019</v>
+        <v>-114174.50657500359</v>
       </c>
     </row>
     <row r="220"/>
@@ -45078,19 +45078,19 @@
         <v>2.4841193830000003</v>
       </c>
       <c r="D236" s="165">
-        <v>0.1978715415</v>
+        <v>0.1922796539</v>
       </c>
       <c r="E236" s="165">
-        <v>-2.2862478415000003</v>
+        <v>-2.2918397291000003</v>
       </c>
       <c r="F236" s="165">
         <v>2.1610657892</v>
       </c>
       <c r="G236" s="165">
-        <v>0.1511573229</v>
+        <v>0.1678268238</v>
       </c>
       <c r="H236" s="165">
-        <v>-2.0099084662999998</v>
+        <v>-1.9932389653999998</v>
       </c>
     </row>
     <row r="237">
@@ -45101,19 +45101,19 @@
         <v>0.060052400808930366</v>
       </c>
       <c r="D237" s="182">
-        <v>0.09090841220715834</v>
+        <v>0.088339323094579161</v>
       </c>
       <c r="E237" s="182">
-        <v>0.030856011398227974</v>
+        <v>0.028286922285648795</v>
       </c>
       <c r="F237" s="182">
         <v>0.05280122907758325</v>
       </c>
       <c r="G237" s="182">
-        <v>0.069446430316123839</v>
+        <v>0.0771049235366095</v>
       </c>
       <c r="H237" s="182">
-        <v>0.016645201238540588</v>
+        <v>0.024303694459026248</v>
       </c>
     </row>
     <row r="238">
@@ -45902,19 +45902,19 @@
         <v>1.108447388735532</v>
       </c>
       <c r="D272" s="182">
-        <v>0.14617871372265667</v>
+        <v>0.14363286112490342</v>
       </c>
       <c r="E272" s="182">
-        <v>-0.96226867501287527</v>
+        <v>-0.96481452761062858</v>
       </c>
       <c r="F272" s="182">
         <v>1.1100487626103262</v>
       </c>
       <c r="G272" s="182">
-        <v>0.21237297437734035</v>
+        <v>0.21893204085535192</v>
       </c>
       <c r="H272" s="182">
-        <v>-0.89767578823298577</v>
+        <v>-0.89111672175497425</v>
       </c>
     </row>
     <row r="273"/>
@@ -47274,16 +47274,16 @@
         <v>1141.5356260585909</v>
       </c>
       <c r="F342" s="59">
-        <v>-65.2926226744237</v>
+        <v>-65.4712264535741</v>
       </c>
       <c r="G342" s="59">
-        <v>-55.9003593069075</v>
+        <v>-54.5934007592003</v>
       </c>
       <c r="H342" s="59">
-        <v>-55.1129366734636</v>
+        <v>-52.4549844144693</v>
       </c>
       <c r="I342" s="59">
-        <v>-54.9396607874432</v>
+        <v>-51.279658446457894</v>
       </c>
       <c r="J342" s="59"/>
       <c r="K342" s="59"/>
@@ -47371,10 +47371,10 @@
         <v>1328</v>
       </c>
       <c r="D359" s="56">
-        <v>72.788947137546614</v>
+        <v>72.610343358396108</v>
       </c>
       <c r="E359" s="57">
-        <v>-94.518904583016067</v>
+        <v>-94.532353662771371</v>
       </c>
     </row>
     <row r="360">
@@ -47413,10 +47413,10 @@
         <v>20</v>
       </c>
       <c r="D362" s="56">
-        <v>22.843482734371641</v>
+        <v>22.664878955221134</v>
       </c>
       <c r="E362" s="57">
-        <v>14.217413671858203</v>
+        <v>13.32439477610567</v>
       </c>
     </row>
     <row r="363">
@@ -47441,10 +47441,10 @@
         <v>1154</v>
       </c>
       <c r="D364" s="56">
-        <v>-65.292622674423711</v>
+        <v>-65.471226453574218</v>
       </c>
       <c r="E364" s="57">
-        <v>-105.65793957317364</v>
+        <v>-105.67341650377593</v>
       </c>
     </row>
     <row r="365">
@@ -47500,7 +47500,7 @@
         <v>10.5</v>
       </c>
       <c r="E368" s="57">
-        <v>-94.518904583016067</v>
+        <v>-94.532353662771371</v>
       </c>
     </row>
     <row r="369">
@@ -47521,10 +47521,10 @@
         <v>58</v>
       </c>
       <c r="D370" s="56">
-        <v>-184.8664790477693</v>
+        <v>-184.90155618637721</v>
       </c>
       <c r="E370" s="57">
-        <v>-418.73530870305052</v>
+        <v>-418.79578652823659</v>
       </c>
     </row>
     <row r="371">
@@ -47535,10 +47535,10 @@
         <v>237</v>
       </c>
       <c r="D371" s="56">
-        <v>-756.426143626655</v>
+        <v>-756.5696702671969</v>
       </c>
       <c r="E371" s="57">
-        <v>-419.16714920955906</v>
+        <v>-419.2277089735008</v>
       </c>
     </row>
     <row r="373">
@@ -47569,7 +47569,7 @@
       </c>
       <c r="C375" s="56"/>
       <c r="D375" s="56">
-        <v>265.61927085571261</v>
+        <v>273.06558022424889</v>
       </c>
       <c r="E375" s="57"/>
     </row>
@@ -47599,7 +47599,7 @@
       </c>
       <c r="C378" s="56"/>
       <c r="D378" s="56">
-        <v>70.382396229797621</v>
+        <v>77.8287055983339</v>
       </c>
       <c r="E378" s="57"/>
     </row>
@@ -47619,7 +47619,7 @@
       </c>
       <c r="C380" s="56"/>
       <c r="D380" s="56">
-        <v>-231.24557944223807</v>
+        <v>-223.79927007370179</v>
       </c>
       <c r="E380" s="57"/>
     </row>
@@ -47677,7 +47677,7 @@
       </c>
       <c r="C386" s="56"/>
       <c r="D386" s="56">
-        <v>-733.58877145802387</v>
+        <v>-732.12634313159015</v>
       </c>
       <c r="E386" s="57"/>
     </row>
@@ -47687,7 +47687,7 @@
       </c>
       <c r="C387" s="56"/>
       <c r="D387" s="56">
-        <v>-3001.6568079842145</v>
+        <v>-2995.6729269421121</v>
       </c>
       <c r="E387" s="57"/>
     </row>

</xml_diff>